<commit_message>
Final for first trial.
</commit_message>
<xml_diff>
--- a/MemoryMap/IO_Mapping.xlsx
+++ b/MemoryMap/IO_Mapping.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A71B6CA-5CE9-41B5-B944-C1FF5DD6C35C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D8C40E-8D03-44CC-B73D-DDFAFEE00AF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="160">
   <si>
     <t>PLC</t>
   </si>
@@ -509,6 +509,9 @@
   <si>
     <t>14KL</t>
   </si>
+  <si>
+    <t>13KR</t>
+  </si>
 </sst>
 </file>
 
@@ -537,7 +540,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -548,12 +551,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -625,20 +622,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5792,7 +5789,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11439525" y="5591175"/>
+          <a:off x="11613460" y="5591175"/>
           <a:ext cx="152400" cy="10487025"/>
           <a:chOff x="5269800" y="0"/>
           <a:chExt cx="152400" cy="7560000"/>
@@ -6041,7 +6038,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2400300" y="5524500"/>
+          <a:off x="2429289" y="5524500"/>
           <a:ext cx="180975" cy="10496550"/>
           <a:chOff x="5255513" y="0"/>
           <a:chExt cx="180975" cy="7560000"/>
@@ -6737,7 +6734,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4413250" y="3533775"/>
+          <a:off x="4480891" y="3533775"/>
           <a:ext cx="6029325" cy="704850"/>
           <a:chOff x="2331338" y="3427575"/>
           <a:chExt cx="6029325" cy="704850"/>
@@ -7059,7 +7056,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8655050" y="11763375"/>
+          <a:off x="8790333" y="11763375"/>
           <a:ext cx="2600325" cy="752475"/>
           <a:chOff x="4045838" y="3403762"/>
           <a:chExt cx="2600325" cy="752475"/>
@@ -7322,7 +7319,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4333863" y="10147302"/>
+          <a:off x="4401504" y="10147302"/>
           <a:ext cx="2098667" cy="774690"/>
           <a:chOff x="4118852" y="3386302"/>
           <a:chExt cx="2098667" cy="774690"/>
@@ -7577,7 +7574,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2628911" y="10172705"/>
+          <a:off x="2667563" y="10172705"/>
           <a:ext cx="1800224" cy="758825"/>
           <a:chOff x="4445899" y="3378368"/>
           <a:chExt cx="1800224" cy="758825"/>
@@ -8938,7 +8935,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1574800" y="5562600"/>
+          <a:off x="1594126" y="5562600"/>
           <a:ext cx="1562100" cy="6638925"/>
           <a:chOff x="4564950" y="460538"/>
           <a:chExt cx="1562100" cy="6638925"/>
@@ -9457,7 +9454,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3267064" y="11670743"/>
+          <a:off x="3315379" y="11670743"/>
           <a:ext cx="1882781" cy="876859"/>
           <a:chOff x="4450637" y="3279381"/>
           <a:chExt cx="2824171" cy="876859"/>
@@ -11488,7 +11485,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5657855" y="11497023"/>
+          <a:off x="5744822" y="11497023"/>
           <a:ext cx="2658993" cy="1056931"/>
           <a:chOff x="4045842" y="3146935"/>
           <a:chExt cx="2658993" cy="1056931"/>
@@ -12279,8 +12276,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2705100" y="8001001"/>
-          <a:ext cx="1797050" cy="1003300"/>
+          <a:off x="2743752" y="8001001"/>
+          <a:ext cx="1826039" cy="1003300"/>
           <a:chOff x="18403017" y="8195094"/>
           <a:chExt cx="3270850" cy="2012831"/>
         </a:xfrm>
@@ -12527,8 +12524,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11321668" y="9088101"/>
-          <a:ext cx="1867287" cy="842807"/>
+          <a:off x="11495603" y="9088101"/>
+          <a:ext cx="1896276" cy="842807"/>
           <a:chOff x="13226668" y="8110201"/>
           <a:chExt cx="1810137" cy="906307"/>
         </a:xfrm>
@@ -43853,8 +43850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C74" sqref="C71:C74"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43867,10 +43864,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="9"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -43897,13 +43894,13 @@
       <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="11">
         <v>3</v>
       </c>
       <c r="B3" s="7">
         <v>1</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -43920,11 +43917,11 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="7">
         <v>2</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -43941,11 +43938,11 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="7">
         <v>3</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -43962,7 +43959,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -43971,7 +43968,7 @@
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="11">
         <v>7</v>
       </c>
       <c r="B7" s="7">
@@ -43986,11 +43983,11 @@
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="7">
         <v>2</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="9" t="s">
         <v>158</v>
       </c>
       <c r="D8" s="7"/>
@@ -43999,7 +43996,7 @@
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="7">
         <v>3</v>
       </c>
@@ -44012,11 +44009,11 @@
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="7">
         <v>4</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="7" t="s">
@@ -44033,12 +44030,12 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="7">
         <v>5</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>16</v>
+        <v>159</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>19</v>
@@ -44054,11 +44051,11 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="7">
         <v>6</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="8">
         <v>19</v>
       </c>
       <c r="D12" s="7" t="s">
@@ -44075,11 +44072,11 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="7">
         <v>7</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="8">
         <v>18</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -44096,11 +44093,11 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="7">
         <v>8</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="7" t="s">
@@ -44117,7 +44114,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="7">
         <v>9</v>
       </c>
@@ -44130,11 +44127,11 @@
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="7">
         <v>10</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D16" s="7" t="s">
@@ -44151,11 +44148,11 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="7">
         <v>11</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="8" t="s">
         <v>32</v>
       </c>
       <c r="D17" s="7" t="s">
@@ -44172,11 +44169,11 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="7">
         <v>12</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="8">
         <v>20</v>
       </c>
       <c r="D18" s="7" t="s">
@@ -44193,11 +44190,11 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="7">
         <v>13</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="8">
         <v>21</v>
       </c>
       <c r="D19" s="7" t="s">
@@ -44214,11 +44211,11 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="7">
         <v>14</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="8">
         <v>17</v>
       </c>
       <c r="D20" s="7" t="s">
@@ -44235,7 +44232,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -44244,7 +44241,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -44253,13 +44250,13 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+      <c r="A23" s="11">
         <v>8</v>
       </c>
       <c r="B23" s="7">
         <v>1</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="8" t="s">
         <v>41</v>
       </c>
       <c r="D23" s="7" t="s">
@@ -44276,11 +44273,11 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="7">
         <v>2</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D24" s="7" t="s">
@@ -44297,11 +44294,11 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="7">
         <v>3</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="8" t="s">
         <v>47</v>
       </c>
       <c r="D25" s="7" t="s">
@@ -44318,11 +44315,11 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="7">
         <v>4</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="8" t="s">
         <v>50</v>
       </c>
       <c r="D26" s="7" t="s">
@@ -44339,11 +44336,11 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
+      <c r="A27" s="11"/>
       <c r="B27" s="7">
         <v>5</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="8" t="s">
         <v>53</v>
       </c>
       <c r="D27" s="7" t="s">
@@ -44360,11 +44357,11 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="7">
         <v>6</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="8" t="s">
         <v>56</v>
       </c>
       <c r="D28" s="7" t="s">
@@ -44381,11 +44378,11 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="7">
         <v>7</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="8" t="s">
         <v>59</v>
       </c>
       <c r="D29" s="7" t="s">
@@ -44402,11 +44399,11 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="7">
         <v>8</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="8" t="s">
         <v>62</v>
       </c>
       <c r="D30" s="7" t="s">
@@ -44423,11 +44420,11 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="7">
         <v>9</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="8">
         <v>19.399999999999999</v>
       </c>
       <c r="D31" s="7" t="s">
@@ -44444,11 +44441,11 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="7">
         <v>10</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C32" s="8">
         <v>19.2</v>
       </c>
       <c r="D32" s="7" t="s">
@@ -44465,11 +44462,11 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="7">
         <v>11</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="8">
         <v>19.3</v>
       </c>
       <c r="D33" s="7" t="s">
@@ -44486,11 +44483,11 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="7">
         <v>12</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="8">
         <v>19.100000000000001</v>
       </c>
       <c r="D34" s="7" t="s">
@@ -44507,11 +44504,11 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="7">
         <v>13</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D35" s="7" t="s">
@@ -44528,11 +44525,11 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
+      <c r="A36" s="11"/>
       <c r="B36" s="7">
         <v>14</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D36" s="7" t="s">
@@ -44549,11 +44546,11 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="7">
         <v>15</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="8" t="s">
         <v>79</v>
       </c>
       <c r="D37" s="7" t="s">
@@ -44570,11 +44567,11 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
+      <c r="A38" s="11"/>
       <c r="B38" s="7">
         <v>16</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="8" t="s">
         <v>82</v>
       </c>
       <c r="D38" s="7" t="s">
@@ -44591,7 +44588,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
+      <c r="A39" s="11"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -44623,13 +44620,13 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="8">
+      <c r="A41" s="11">
         <v>12</v>
       </c>
       <c r="B41" s="7">
         <v>1</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D41" s="7" t="s">
@@ -44646,7 +44643,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
+      <c r="A42" s="11"/>
       <c r="B42" s="7">
         <v>2</v>
       </c>
@@ -44659,11 +44656,11 @@
       <c r="G42" s="7"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
+      <c r="A43" s="11"/>
       <c r="B43" s="7">
         <v>3</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="8" t="s">
         <v>89</v>
       </c>
       <c r="D43" s="7" t="s">
@@ -44680,11 +44677,11 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
+      <c r="A44" s="11"/>
       <c r="B44" s="7">
         <v>4</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="8" t="s">
         <v>92</v>
       </c>
       <c r="D44" s="7" t="s">
@@ -44701,7 +44698,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
+      <c r="A45" s="11"/>
       <c r="B45" s="7">
         <v>5</v>
       </c>
@@ -44714,7 +44711,7 @@
       <c r="G45" s="7"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="8"/>
+      <c r="A46" s="11"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7">
         <v>47</v>
@@ -44725,7 +44722,7 @@
       <c r="G46" s="7"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
+      <c r="A47" s="11"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
@@ -44734,7 +44731,7 @@
       <c r="G47" s="7"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="8"/>
+      <c r="A48" s="11"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
@@ -44743,7 +44740,7 @@
       <c r="G48" s="7"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
+      <c r="A49" s="11"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
@@ -44752,7 +44749,7 @@
       <c r="G49" s="7"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="8">
+      <c r="A50" s="11">
         <v>13</v>
       </c>
       <c r="B50" s="7">
@@ -44767,7 +44764,7 @@
       <c r="G50" s="7"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="8"/>
+      <c r="A51" s="11"/>
       <c r="B51" s="7">
         <v>2</v>
       </c>
@@ -44780,11 +44777,11 @@
       <c r="G51" s="7"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="8"/>
+      <c r="A52" s="11"/>
       <c r="B52" s="7">
         <v>3</v>
       </c>
-      <c r="C52" s="11">
+      <c r="C52" s="8">
         <v>57</v>
       </c>
       <c r="D52" s="7" t="s">
@@ -44801,7 +44798,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="8"/>
+      <c r="A53" s="11"/>
       <c r="B53" s="7">
         <v>4</v>
       </c>
@@ -44814,11 +44811,11 @@
       <c r="G53" s="7"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="8"/>
+      <c r="A54" s="11"/>
       <c r="B54" s="7">
         <v>5</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="8" t="s">
         <v>101</v>
       </c>
       <c r="D54" s="7" t="s">
@@ -44835,11 +44832,11 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="8"/>
+      <c r="A55" s="11"/>
       <c r="B55" s="7">
         <v>6</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C55" s="8" t="s">
         <v>104</v>
       </c>
       <c r="D55" s="7" t="s">
@@ -44856,7 +44853,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="8"/>
+      <c r="A56" s="11"/>
       <c r="B56" s="7">
         <v>7</v>
       </c>
@@ -44869,7 +44866,7 @@
       <c r="G56" s="7"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="8"/>
+      <c r="A57" s="11"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
@@ -44901,13 +44898,13 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="8">
+      <c r="A59" s="11">
         <v>9</v>
       </c>
       <c r="B59" s="7">
         <v>1</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="8" t="s">
         <v>108</v>
       </c>
       <c r="D59" s="7" t="s">
@@ -44924,11 +44921,11 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="8"/>
+      <c r="A60" s="11"/>
       <c r="B60" s="7">
         <v>2</v>
       </c>
-      <c r="C60" s="11">
+      <c r="C60" s="8">
         <v>32</v>
       </c>
       <c r="D60" s="7" t="s">
@@ -44945,11 +44942,11 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="8"/>
+      <c r="A61" s="11"/>
       <c r="B61" s="7">
         <v>3</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="C61" s="8" t="s">
         <v>113</v>
       </c>
       <c r="D61" s="7" t="s">
@@ -44966,11 +44963,11 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="8"/>
+      <c r="A62" s="11"/>
       <c r="B62" s="7">
         <v>4</v>
       </c>
-      <c r="C62" s="11" t="s">
+      <c r="C62" s="8" t="s">
         <v>116</v>
       </c>
       <c r="D62" s="7" t="s">
@@ -44987,11 +44984,11 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="8"/>
+      <c r="A63" s="11"/>
       <c r="B63" s="7">
         <v>5</v>
       </c>
-      <c r="C63" s="11" t="s">
+      <c r="C63" s="8" t="s">
         <v>119</v>
       </c>
       <c r="D63" s="7" t="s">
@@ -45008,11 +45005,11 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="8"/>
+      <c r="A64" s="11"/>
       <c r="B64" s="7">
         <v>6</v>
       </c>
-      <c r="C64" s="11" t="s">
+      <c r="C64" s="8" t="s">
         <v>122</v>
       </c>
       <c r="D64" s="7" t="s">
@@ -45029,7 +45026,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="8"/>
+      <c r="A65" s="11"/>
       <c r="B65" s="7">
         <v>7</v>
       </c>
@@ -45042,11 +45039,11 @@
       <c r="G65" s="7"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="8"/>
+      <c r="A66" s="11"/>
       <c r="B66" s="7">
         <v>8</v>
       </c>
-      <c r="C66" s="11">
+      <c r="C66" s="8">
         <v>38</v>
       </c>
       <c r="D66" s="7" t="s">
@@ -45063,11 +45060,11 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="8"/>
+      <c r="A67" s="11"/>
       <c r="B67" s="7">
         <v>9</v>
       </c>
-      <c r="C67" s="11" t="s">
+      <c r="C67" s="8" t="s">
         <v>128</v>
       </c>
       <c r="D67" s="7" t="s">
@@ -45084,11 +45081,11 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="8"/>
+      <c r="A68" s="11"/>
       <c r="B68" s="7">
         <v>10</v>
       </c>
-      <c r="C68" s="11">
+      <c r="C68" s="8">
         <v>33</v>
       </c>
       <c r="D68" s="7" t="s">
@@ -45105,11 +45102,11 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="8"/>
+      <c r="A69" s="11"/>
       <c r="B69" s="7">
         <v>11</v>
       </c>
-      <c r="C69" s="11" t="s">
+      <c r="C69" s="8" t="s">
         <v>131</v>
       </c>
       <c r="D69" s="7" t="s">
@@ -45126,7 +45123,7 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="8"/>
+      <c r="A70" s="11"/>
       <c r="B70" s="7">
         <v>12</v>
       </c>
@@ -45139,11 +45136,11 @@
       <c r="G70" s="7"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="8"/>
+      <c r="A71" s="11"/>
       <c r="B71" s="7">
         <v>13</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="C71" s="8" t="s">
         <v>135</v>
       </c>
       <c r="D71" s="7" t="s">
@@ -45160,11 +45157,11 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="8"/>
+      <c r="A72" s="11"/>
       <c r="B72" s="7">
         <v>14</v>
       </c>
-      <c r="C72" s="11" t="s">
+      <c r="C72" s="8" t="s">
         <v>138</v>
       </c>
       <c r="D72" s="7" t="s">
@@ -45181,11 +45178,11 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="8"/>
+      <c r="A73" s="11"/>
       <c r="B73" s="7">
         <v>15</v>
       </c>
-      <c r="C73" s="11">
+      <c r="C73" s="8">
         <v>36</v>
       </c>
       <c r="D73" s="7" t="s">
@@ -45202,11 +45199,11 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="8"/>
+      <c r="A74" s="11"/>
       <c r="B74" s="7">
         <v>16</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="C74" s="8" t="s">
         <v>143</v>
       </c>
       <c r="D74" s="7" t="s">
@@ -45246,7 +45243,7 @@
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="8">
+      <c r="A76" s="11">
         <v>16</v>
       </c>
       <c r="B76" s="7">
@@ -45261,7 +45258,7 @@
       <c r="G76" s="7"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="8"/>
+      <c r="A77" s="11"/>
       <c r="B77" s="7">
         <v>2</v>
       </c>
@@ -45274,11 +45271,11 @@
       <c r="G77" s="7"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="8"/>
+      <c r="A78" s="11"/>
       <c r="B78" s="7">
         <v>3</v>
       </c>
-      <c r="C78" s="11" t="s">
+      <c r="C78" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D78" s="7" t="s">
@@ -45295,11 +45292,11 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="8"/>
+      <c r="A79" s="11"/>
       <c r="B79" s="7">
         <v>4</v>
       </c>
-      <c r="C79" s="11" t="s">
+      <c r="C79" s="8" t="s">
         <v>149</v>
       </c>
       <c r="D79" s="7" t="s">
@@ -45316,7 +45313,7 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="8"/>
+      <c r="A80" s="11"/>
       <c r="B80" s="7">
         <v>5</v>
       </c>
@@ -45329,11 +45326,11 @@
       <c r="G80" s="7"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="8"/>
+      <c r="A81" s="11"/>
       <c r="B81" s="7">
         <v>6</v>
       </c>
-      <c r="C81" s="11">
+      <c r="C81" s="8">
         <v>61</v>
       </c>
       <c r="D81" s="7" t="s">
@@ -45350,7 +45347,7 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="8">
+      <c r="A82" s="11">
         <v>22</v>
       </c>
       <c r="B82" s="7">
@@ -45365,7 +45362,7 @@
       <c r="G82" s="7"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="8"/>
+      <c r="A83" s="11"/>
       <c r="B83" s="7">
         <v>2</v>
       </c>
@@ -45378,7 +45375,7 @@
       <c r="G83" s="7"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="8"/>
+      <c r="A84" s="11"/>
       <c r="B84" s="7">
         <v>3</v>
       </c>
@@ -45389,7 +45386,7 @@
       <c r="G84" s="7"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="8"/>
+      <c r="A85" s="11"/>
       <c r="B85" s="7">
         <v>4</v>
       </c>
@@ -45400,7 +45397,7 @@
       <c r="G85" s="7"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="8"/>
+      <c r="A86" s="11"/>
       <c r="B86" s="7">
         <v>5</v>
       </c>
@@ -46513,7 +46510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X87"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="E30" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>

</xml_diff>